<commit_message>
Changes in Intelligent Automation page
</commit_message>
<xml_diff>
--- a/ResponsesData/mChat Responses.xlsx
+++ b/ResponsesData/mChat Responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASA CHATBOT\mChat-RASA\ResponsesData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FA2A78-6357-414D-B8BD-2FFAFD63C592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B164CE1-4AA4-43AF-8EC2-9BBDC21FB73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C305AD81-7B09-4460-9FA4-D61D86DA96BD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="189">
   <si>
     <t>Response Name</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Hi, \nWelcome to Marlabs Website.\nI'm &lt;b&gt;mChat&lt;/b&gt;, \nHow can I help you today with your queries?</t>
-  </si>
-  <si>
-    <t>Events&amp;Webinar:https://www.marlabs.com/events-webinars/, Careers:https://www.marlabs.com/careers/, Intellegent Automation:https://www.marlabs.com/intelligent-automation/, Intellegent Experience:https://www.marlabs.com/intelligent-experiences/, Divergence:https://www.marlabs.com/divergence/</t>
   </si>
   <si>
     <t>From past 25 years we have been providing best solutions to our client with our strengths in Rich Capabilities Mix, Speed and Nimbleness, Empathy-fueled Drive and Powerful Ecosystem.</t>
@@ -493,9 +490,6 @@
     <t>Machine learning is a branch of artificial intelligence (AI) and computer science which focuses on the use of data and algorithms to imitate the way that humans learn, gradually improving its accuracy.</t>
   </si>
   <si>
-    <t>Purpose:/ML_Purpose_In_PA, Usages:/How_ML_Used_In_PA</t>
-  </si>
-  <si>
     <t>action_utter_How_ML_Used_In_PA</t>
   </si>
   <si>
@@ -610,6 +604,63 @@
   </si>
   <si>
     <t>action_utter_PRE_Disadvantages</t>
+  </si>
+  <si>
+    <t>Visit Website: https://www.marlabs.com/intelligent-automation/</t>
+  </si>
+  <si>
+    <t>Fuzzy logic in AI:/FL_AI</t>
+  </si>
+  <si>
+    <t>Click the button to know more,</t>
+  </si>
+  <si>
+    <t>Events &amp; Webinar:https://www.marlabs.com/events-webinars/, Careers:https://www.marlabs.com/careers/, Intelligent Experience:https://www.marlabs.com/intelligent-experiences/, Divergence:https://www.marlabs.com/divergence/</t>
+  </si>
+  <si>
+    <t>action_utter_RPA_Design_Implementation_Topics</t>
+  </si>
+  <si>
+    <t>Select any topic to know more,</t>
+  </si>
+  <si>
+    <t>Benefits:/API_Benefits, API Security:/ API_Security,API Performance:/API_Performance,API enabling system:/API_Enable, API driven process:/API_Driven, API endpoint:/API_EndPoint</t>
+  </si>
+  <si>
+    <t>Process discovery:/PD_Definition, Process mining:/PM_Definition,Process re-engineering:/PRE_Definition,API-enabling system driven process end-points:/API,Experts in industry-leading RPA products and platforms:/How_Marlabs_Expert</t>
+  </si>
+  <si>
+    <t>Recognitions:/Marlabs_Recognition, Our best products:/Marlabs_Best_Products,Solution areas:/Marlabs_Solution_Area</t>
+  </si>
+  <si>
+    <t>Visit Website: https://www.marlabs.com/intelligent-automation/#fws_62e0d9b811ce8</t>
+  </si>
+  <si>
+    <t>Purpose:/ML_Purpose_In_PA, Usages:/How_ML_Used_In_PA,Process analyticsTypes:/PA_Types</t>
+  </si>
+  <si>
+    <t>Process analyticsTypes:/PA_Types</t>
+  </si>
+  <si>
+    <t>Descriptive Analytics:/Descriptive_PA_Definition ,Predictive Analytics:/Predictive_PA_Definition, Prescriptive Analytics:/Prescriptive_PA_Definition</t>
+  </si>
+  <si>
+    <t>RPA Bot as service:/AI_RPA_bot,Intelligent Automation:/AI_IA</t>
+  </si>
+  <si>
+    <t>ML-powered process analytics:/ML_Definition,AI automation bots as a service:/AI_bot_service,Computer Vision:/CV_Definition,NLP:/NLP_Definition,Fuzzy logic:/FL_Definition,Digital assistants:/DA_Definition,Chatbots:/Chatbot_Definition</t>
+  </si>
+  <si>
+    <t>action_utter_Intelligent_Automation</t>
+  </si>
+  <si>
+    <t>RPA Design &amp; Implementation:/RPA_Design_Implementation_Topics, Intelligent Automation:/Intelligent_Automation_Topics</t>
+  </si>
+  <si>
+    <t>action_utter_Intelligent_Automation_Topics</t>
+  </si>
+  <si>
+    <t>Intelligent Automation:/Intelligent_Automation</t>
   </si>
 </sst>
 </file>
@@ -672,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -688,6 +739,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,17 +1057,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47F5EE0-A80F-4F83-BB66-CB97BAE0C58E}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="79.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="39" style="3" customWidth="1"/>
     <col min="4" max="4" width="67.85546875" style="3" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -1033,659 +1087,718 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C6" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="8" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
+      <c r="C11" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>63</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3" t="s">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="3" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="3" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="C25" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>81</v>
+      <c r="C35" s="3" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C39" s="3" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B40" s="3" t="s">
+    </row>
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="3" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="3" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="B46" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="3" t="s">
+    </row>
+    <row r="47" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C48" s="3" t="s">
+    </row>
+    <row r="52" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="C52" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C57" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="3" t="s">
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="3" t="s">
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B57" s="3" t="s">
+    </row>
+    <row r="61" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="B61" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B58" s="3" t="s">
+    </row>
+    <row r="62" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="B62" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C62" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="C67" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="69" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B69" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+    <row r="70" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B70" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+    <row r="72" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B69" s="3" t="s">
+    </row>
+    <row r="73" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+    <row r="74" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+    <row r="75" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B71" s="3" t="s">
+    </row>
+    <row r="76" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B72" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+    <row r="77" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B74" s="3" t="s">
+    </row>
+    <row r="78" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for some responses
</commit_message>
<xml_diff>
--- a/ResponsesData/mChat Responses.xlsx
+++ b/ResponsesData/mChat Responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASA CHATBOT\mChat-RASA\ResponsesData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF07A3F-ECB1-4D3B-B4EC-E339D6C37556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BEC5B7-30F3-4E38-B12F-DCC8075F7434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C305AD81-7B09-4460-9FA4-D61D86DA96BD}"/>
   </bookViews>
@@ -305,9 +305,6 @@
     <t>Intelligent Automation (IA) is a combination of Robotic Process Automation (RPA) and artificial intelligence (AI) technologies which together empower rapid end-to-end business process automation and accelerate digital transformation.</t>
   </si>
   <si>
-    <t>action_utter_AI_Aiaas</t>
-  </si>
-  <si>
     <t>AIaas stands for Artificial Intelligence as a service</t>
   </si>
   <si>
@@ -347,23 +344,7 @@
     <t>action_utter_AI_DisAdvantages</t>
   </si>
   <si>
-    <t>&lt;li&gt; Expensive&lt;/li&gt;	                                                                       &lt;li&gt;Requires deep technical expertise &lt;/li&gt;                                    &lt;li&gt;Limited supply of qualified workers to build AI tools&lt;/li&gt;
-&lt;li&gt;Only knows what it's been shown; and&lt;/li&gt;
-&lt;li&gt;Lack of ability to generalize from one task to another.&lt;/li&gt;</t>
-  </si>
-  <si>
     <t>Advantages:/AI_Advantages,Benefits:/AI_Benefits</t>
-  </si>
-  <si>
-    <t>action_ utter_AI_Benefits</t>
-  </si>
-  <si>
-    <t>&lt;li&gt;Chatbots use AI to understand customer problems faster and provide more efficient answers&lt;/li&gt;
-&lt;li&gt;Intelligent assistants use AI to parse critical information from large free-text datasets to improve scheduling&lt;/li&gt;
-&lt;li&gt;Recommendation engines can provide automated recommendations for TV shows based on users viewing habits&lt;/li&gt;</t>
-  </si>
-  <si>
-    <t>action_ utter_AI_Technology</t>
   </si>
   <si>
     <t>Intelligent Automation (IA) is a combination of Robotic Process Automation (RPA) and artificial intelligence (AI) technologies together.</t>
@@ -633,9 +614,6 @@
     <t>Visit Website: https://www.marlabs.com/intelligent-automation/#fws_62e0d9b811ce8</t>
   </si>
   <si>
-    <t>Purpose:/ML_Purpose_In_PA, Usages:/How_ML_Used_In_PA,Process analyticsTypes:/PA_Types</t>
-  </si>
-  <si>
     <t>Process analyticsTypes:/PA_Types</t>
   </si>
   <si>
@@ -661,6 +639,28 @@
   </si>
   <si>
     <t>Stages:/PRE_Stages, Benefits:/PRE_Benefits, Disadvantages:/PRE_Disadvantages</t>
+  </si>
+  <si>
+    <t>action_utter_AI_Benefits</t>
+  </si>
+  <si>
+    <t>action_utter_AI_Technology</t>
+  </si>
+  <si>
+    <t>These are the Benefits:&lt;li&gt;Chatbots use AI to understand customer problems faster and provide more efficient answers&lt;/li&gt;
+&lt;li&gt;Intelligent assistants use AI to parse critical information from large free-text datasets to improve scheduling&lt;/li&gt;
+&lt;li&gt;Recommendation engines can provide automated recommendations for TV shows based on users viewing habits&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>These are the Disadvantages:&lt;li&gt; Expensive&lt;/li&gt;	                                                                       &lt;li&gt;Requires deep technical expertise &lt;/li&gt;                                    &lt;li&gt;Limited supply of qualified workers to build AI tools&lt;/li&gt;
+&lt;li&gt;Only knows what it's been shown&lt;/li&gt;
+&lt;li&gt;Lack of ability to generalize from one task to another.&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Purpose:/ML_Purpose_In_PA, Usages:/How_ML_Used_In_PA,Process analytics types:/PA_Types</t>
+  </si>
+  <si>
+    <t>action_utter_AI_AIaas</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47F5EE0-A80F-4F83-BB66-CB97BAE0C58E}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,44 +1088,44 @@
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1136,10 +1136,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,7 +1274,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>73</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1463,342 +1463,342 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>92</v>
+      <c r="C43" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C44" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>101</v>
+        <v>183</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>103</v>
+        <v>184</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new changes done suggested by Jareeb
</commit_message>
<xml_diff>
--- a/ResponsesData/mChat Responses.xlsx
+++ b/ResponsesData/mChat Responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASA CHATBOT\mChat-RASA\ResponsesData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ADE400-7B19-48C6-BA43-3086268C8E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17579A38-6D39-4580-A8B9-D7478536D731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C305AD81-7B09-4460-9FA4-D61D86DA96BD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="191">
   <si>
     <t>Response Name</t>
   </si>
@@ -224,9 +224,6 @@
     <t>RPA Chatbot:/Chatbot_RPA, Benefits:/Chatbot_Benefits</t>
   </si>
   <si>
-    <t>Workings:/PD_Working, Benefits:/PD_Benefits</t>
-  </si>
-  <si>
     <t>Usage:/PM_Usage,Benefits:/PM_Benefits</t>
   </si>
   <si>
@@ -590,13 +587,7 @@
     <t>Fuzzy logic in AI:/FL_AI</t>
   </si>
   <si>
-    <t>Click the button to know more,</t>
-  </si>
-  <si>
     <t>action_utter_RPA_Design_Implementation_Topics</t>
-  </si>
-  <si>
-    <t>Select any topic to know more,</t>
   </si>
   <si>
     <t>Benefits:/API_Benefits, API Security:/ API_Security,API Performance:/API_Performance,API enabling system:/API_Enable, API driven process:/API_Driven, API endpoint:/API_EndPoint</t>
@@ -670,6 +661,12 @@
   </si>
   <si>
     <t>Intelligent Experience:https://www.marlabs.com/intelligent-experiences/,Cloud powered IT Modernization:https://www.marlabs.com/cloud-powered-it-modernization/,Cybersecurity &amp; Privacy:https://www.marlabs.com/cybersecurity/,Connected Systems:https://www.marlabs.com/connected-systems/,Data Analytics &amp; AI:https://www.marlabs.com/data-analytics-ai/,Salesforce-powered:https://www.marlabs.com/generate-more-force-from-salesforce/</t>
+  </si>
+  <si>
+    <t>Click any of the button to know more,</t>
+  </si>
+  <si>
+    <t>Process:/PD_Working, Benefits:/PD_Benefits</t>
   </si>
 </sst>
 </file>
@@ -1068,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47F5EE0-A80F-4F83-BB66-CB97BAE0C58E}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,66 +1100,66 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>166</v>
+        <v>189</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>170</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1173,7 +1170,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -1210,13 +1207,13 @@
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1245,7 +1242,7 @@
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>51</v>
@@ -1291,13 +1288,13 @@
     </row>
     <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -1310,7 +1307,7 @@
     </row>
     <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>34</v>
@@ -1337,7 +1334,7 @@
     </row>
     <row r="26" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>39</v>
@@ -1364,13 +1361,13 @@
     </row>
     <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>59</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -1391,13 +1388,13 @@
     </row>
     <row r="32" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1418,410 +1415,410 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="C36" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="C44" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="C45" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="C53" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="C58" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="C65" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="C66" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="C68" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="C73" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New update with Form and dynamic menu
</commit_message>
<xml_diff>
--- a/ResponsesData/mChat Responses.xlsx
+++ b/ResponsesData/mChat Responses.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASA CHATBOT\mChat-RASA\ResponsesData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CB23A5-E817-4AE1-AD8B-76D418A59AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0889C8CA-8721-4EED-A9B2-859BECDBA662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C305AD81-7B09-4460-9FA4-D61D86DA96BD}"/>
   </bookViews>
   <sheets>
     <sheet name="responses" sheetId="1" r:id="rId1"/>
+    <sheet name="forms" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,8 +35,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Keshab Manni</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{BE6721CB-DEF2-46C9-90EA-1E7387D49088}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Keshab Manni:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+{input_name, slot_name,input_type}; {input_name, slot_name, input_type}</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="197">
   <si>
     <t>Response Name</t>
   </si>
@@ -657,23 +692,41 @@
     <t>Digital Solutions:/Digital_Solutions</t>
   </si>
   <si>
-    <t>Divergence:https://www.marlabs.com/divergence/,Our Alliances:https://www.marlabs.com/our-alliances/,Digital Victories:https://www.marlabs.com/digital-victories/,Events &amp; Webinars:https://www.marlabs.com/events-webinars/,Now &amp; Next:https://www.marlabs.com/now-and-next/, Careers:https://www.marlabs.com/careers/</t>
-  </si>
-  <si>
     <t>Intelligent Experience:https://www.marlabs.com/intelligent-experiences/,Cloud powered IT Modernization:https://www.marlabs.com/cloud-powered-it-modernization/,Cybersecurity &amp; Privacy:https://www.marlabs.com/cybersecurity/,Connected Systems:https://www.marlabs.com/connected-systems/,Data Analytics &amp; AI:https://www.marlabs.com/data-analytics-ai/,Salesforce-powered:https://www.marlabs.com/generate-more-force-from-salesforce/</t>
   </si>
   <si>
     <t>Process:/PD_Working, Benefits:/PD_Benefits</t>
   </si>
   <si>
-    <t>Click any of the buttons to know more,</t>
+    <t>action_utter_Main_Menu</t>
+  </si>
+  <si>
+    <t>Please type in your queries or click on any of the topics below,</t>
+  </si>
+  <si>
+    <t>action_utter_Contact_Form</t>
+  </si>
+  <si>
+    <t>Form Title</t>
+  </si>
+  <si>
+    <t>Form Fields</t>
+  </si>
+  <si>
+    <t>Sub Title</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>[Name,user_name,text];[Phone,user_phone,text];[Email,user_email,email];[Query,user_query,text]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,8 +740,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -698,6 +764,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -729,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -747,6 +819,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1063,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47F5EE0-A80F-4F83-BB66-CB97BAE0C58E}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,732 +1170,740 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>190</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="D4" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>165</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>190</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>190</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="25" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="C30" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B34" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="35" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="39" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="45" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="48" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="49" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B50" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="51" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+    <row r="56" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B56" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+    <row r="58" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+    <row r="59" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+    <row r="60" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B62" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+    <row r="63" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B68" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="70" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+    <row r="71" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+    <row r="73" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+    <row r="74" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="77" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+    <row r="78" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+    <row r="79" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1825,4 +1911,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAB6AB0-A972-4333-B192-503AB10465A8}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
NlU intents examples update
</commit_message>
<xml_diff>
--- a/ResponsesData/mChat Responses.xlsx
+++ b/ResponsesData/mChat Responses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mChat\mChat-Rasa\ResponsesData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RASA CHATBOT\mChat-RASA\ResponsesData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C9AB3A-5C6A-4C22-AA1B-FB8AE6D2C693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873CBB99-1F82-4D29-B9E9-8219A8B7252D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="responses" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>action_utter_Digital_Solutions</t>
   </si>
   <si>
-    <t>Intelligent Automation:/Intelligent_Automation</t>
-  </si>
-  <si>
     <t>Intelligent Experience:https://www.marlabs.com/intelligent-experiences/,Cloud powered IT Modernization:https://www.marlabs.com/cloud-powered-it-modernization/,Cybersecurity &amp; Privacy:https://www.marlabs.com/cybersecurity/,Connected Systems:https://www.marlabs.com/connected-systems/,Data Analytics &amp; AI:https://www.marlabs.com/data-analytics-ai/,Salesforce-powered:https://www.marlabs.com/generate-more-force-from-salesforce/</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
   </si>
   <si>
     <t>Natural Language Processing(NLP) helps computers communicate with humans in their own language and scales other language-related tasks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NLP RPA:/NLP_RPA, Application:/NLP_Application</t>
   </si>
   <si>
     <t>action_utter_NLP_RPA</t>
@@ -850,9 +844,6 @@
     <t>Prescriptive PA definition</t>
   </si>
   <si>
-    <t>Process Analytics used areas</t>
-  </si>
-  <si>
     <t>Process Reengineering definition</t>
   </si>
   <si>
@@ -871,15 +862,9 @@
     <t>RPA definition</t>
   </si>
   <si>
-    <t>RPA used areas</t>
-  </si>
-  <si>
     <t>Intelligent Automation Page</t>
   </si>
   <si>
-    <t>Workings:/PD_Working, Benefits:/PD_Benefits</t>
-  </si>
-  <si>
     <t>How Marlabs Industry Leading company?</t>
   </si>
   <si>
@@ -908,6 +893,21 @@
   </si>
   <si>
     <t>API Benefits</t>
+  </si>
+  <si>
+    <t>Intelligent Automation:/Intelligent_Automation_Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NLP in RPA:/NLP_RPA, Applications:/NLP_Application</t>
+  </si>
+  <si>
+    <t>Procedure:/PD_Working, Benefits:/PD_Benefits</t>
+  </si>
+  <si>
+    <t>RPA usage areas</t>
+  </si>
+  <si>
+    <t>Process Analytics usage areas</t>
   </si>
 </sst>
 </file>
@@ -1340,8 +1340,8 @@
   </sheetPr>
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="D68" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,7 +1367,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,943 +1403,943 @@
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="E11" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="E12" s="6" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="E13" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="E15" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="E16" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>47</v>
+      <c r="C17" s="3" t="s">
+        <v>272</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="E19" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="E24" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="E27" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="E33" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="E36" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="E37" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="E38" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="E41" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="E44" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="E45" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="47" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>131</v>
-      </c>
       <c r="E53" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="E54" s="11" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="E59" s="11" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>156</v>
-      </c>
       <c r="E64" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>161</v>
-      </c>
       <c r="E66" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>164</v>
-      </c>
       <c r="E67" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="E69" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E70" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C74" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>180</v>
-      </c>
       <c r="E74" s="11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="75" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="76" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C79" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>191</v>
-      </c>
       <c r="E79" s="11" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>